<commit_message>
excel reader with view
</commit_message>
<xml_diff>
--- a/modules/ExcelReader/src/test/resources/sample.xlsx
+++ b/modules/ExcelReader/src/test/resources/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Actividad</t>
   </si>
@@ -58,9 +58,6 @@
     <t>asdsa</t>
   </si>
   <si>
-    <t>asdas</t>
-  </si>
-  <si>
     <t>qweqweewq</t>
   </si>
   <si>
@@ -74,6 +71,21 @@
   </si>
   <si>
     <t>dweewasdsa</t>
+  </si>
+  <si>
+    <t>11/2022</t>
+  </si>
+  <si>
+    <t>12/2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>04/2024</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
 </sst>
 </file>
@@ -145,13 +157,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,51 +472,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
+    <col min="5" max="5" width="23.875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -508,8 +524,8 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -517,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -525,8 +541,8 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -534,7 +550,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -542,8 +558,8 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>6</v>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -551,7 +567,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -559,8 +575,8 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -568,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -576,12 +592,15 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>4</v>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E10" s="2"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>